<commit_message>
New test scenario 1.19
</commit_message>
<xml_diff>
--- a/OE_IOLMaster_TestScenarios.xlsx
+++ b/OE_IOLMaster_TestScenarios.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james.pels\SharePoint\OpenEyes Intranet - Documents\Team\James\Development\IOL Master Interface\Scenario Test Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james.pels\Documents\OpenEyes\DICOM_test_files\Scenario Test Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="360">
   <si>
     <t>ID</t>
   </si>
@@ -1274,14 +1274,6 @@
 5. When presented with the "select DICOM file" list, check that the blue "I want to add a file manually" link does not display,</t>
   </si>
   <si>
-    <t>PASS</t>
-  </si>
-  <si>
-    <t>All data displayed as expected.
-Able to save correctly.
-Resulting view and edit modes display as expected.</t>
-  </si>
-  <si>
     <t>Biometry data copied to correct fields
 Left eye data in left eye; no data in right eye
 Single formula available in formula drop-down
@@ -1294,44 +1286,10 @@
 All lens power &amp; predictions correct</t>
   </si>
   <si>
-    <t>Handled multiple records and blank calculation locks correctly - no duplicates, no "0/0" records.</t>
-  </si>
-  <si>
-    <t>All correct except "AL difference &gt; 0.3mm" warning shows incorrectly.</t>
-  </si>
-  <si>
-    <t>WARNING</t>
-  </si>
-  <si>
-    <t>Blank lens blocked handled correctly - only lens / formula combos with data displayed.</t>
-  </si>
-  <si>
-    <t>All records merged correctly.</t>
-  </si>
-  <si>
-    <t>"Missing lens data" warning displayed correctly.</t>
-  </si>
-  <si>
-    <t>records merged correctly.
-Initial "missing lens data" not displayed after merge.</t>
-  </si>
-  <si>
-    <t>No change after merging second file.</t>
-  </si>
-  <si>
-    <t>Only one A constant saved for Haigis-L (known limitation)</t>
-  </si>
-  <si>
     <t>Multple files, ACD changes
 1. Base file format (MF/SL)
 followed by
 2. Same file with ACD changed manually</t>
-  </si>
-  <si>
-    <t>invald test - AL is Eval! So no warning should show.</t>
-  </si>
-  <si>
-    <t>Shows "Right AL set manually"</t>
   </si>
   <si>
     <t>Base file format
@@ -1358,6 +1316,11 @@
   </si>
   <si>
     <t>1969-05-15</t>
+  </si>
+  <si>
+    <t>0-1.2.276.0.75.2.1.10.0.2.151215152648562.15295058.31857_0000_000001_14501928990018.dcm
+followed by
+1-1.2.276.0.75.2.1.10.0.2.151215152648562.15295058.31857_0000_000001_14501929230019.dcm</t>
   </si>
 </sst>
 </file>
@@ -1621,15 +1584,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="3" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1647,6 +1601,45 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1668,36 +1661,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2015,11 +1978,11 @@
   </sheetPr>
   <dimension ref="A2:XEZ85"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C26" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E28" sqref="E28"/>
+      <selection pane="bottomRight" activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2030,10 +1993,10 @@
     <col min="4" max="4" width="50.7109375" style="4" customWidth="1"/>
     <col min="5" max="5" width="25.7109375" style="4" customWidth="1"/>
     <col min="6" max="6" width="11.5703125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="5.28515625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="12.140625" style="4" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="5.28515625" style="4" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" style="4" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" style="4" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" style="4" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="9" style="22" customWidth="1"/>
     <col min="12" max="12" width="39.5703125" style="4" customWidth="1"/>
     <col min="13" max="16384" width="9.140625" style="4"/>
@@ -2124,12 +2087,7 @@
       <c r="J5" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="K5" s="23" t="s">
-        <v>349</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>350</v>
-      </c>
+      <c r="K5" s="23"/>
     </row>
     <row r="6" spans="1:12" s="5" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A6" s="16">
@@ -2162,25 +2120,20 @@
       <c r="J6" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="K6" s="23" t="s">
-        <v>349</v>
-      </c>
-      <c r="L6" s="5" t="s">
-        <v>350</v>
-      </c>
+      <c r="K6" s="23"/>
     </row>
     <row r="7" spans="1:12" s="5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="63">
+      <c r="A7" s="50">
         <v>1.3</v>
       </c>
-      <c r="B7" s="61" t="s">
+      <c r="B7" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="61" t="s">
+      <c r="C7" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="61" t="s">
-        <v>351</v>
+      <c r="D7" s="48" t="s">
+        <v>349</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>117</v>
@@ -2200,18 +2153,13 @@
       <c r="J7" s="18">
         <v>27771</v>
       </c>
-      <c r="K7" s="23" t="s">
-        <v>349</v>
-      </c>
-      <c r="L7" s="5" t="s">
-        <v>350</v>
-      </c>
+      <c r="K7" s="23"/>
     </row>
     <row r="8" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="64"/>
-      <c r="B8" s="62"/>
-      <c r="C8" s="62"/>
-      <c r="D8" s="62"/>
+      <c r="A8" s="51"/>
+      <c r="B8" s="49"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="49"/>
       <c r="E8" s="4" t="s">
         <v>118</v>
       </c>
@@ -2229,12 +2177,6 @@
       </c>
       <c r="J8" s="18">
         <v>7980</v>
-      </c>
-      <c r="K8" s="22" t="s">
-        <v>349</v>
-      </c>
-      <c r="L8" s="4" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="9" spans="1:12" s="5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -2268,12 +2210,7 @@
       <c r="J9" s="18">
         <v>15098</v>
       </c>
-      <c r="K9" s="23" t="s">
-        <v>349</v>
-      </c>
-      <c r="L9" s="5" t="s">
-        <v>350</v>
-      </c>
+      <c r="K9" s="23"/>
     </row>
     <row r="10" spans="1:12" s="31" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A10" s="30">
@@ -2293,16 +2230,16 @@
       </c>
     </row>
     <row r="11" spans="1:12" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="55">
+      <c r="A11" s="52">
         <v>1.6</v>
       </c>
-      <c r="B11" s="58" t="s">
+      <c r="B11" s="55" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="58" t="s">
+      <c r="C11" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="58" t="s">
+      <c r="D11" s="55" t="s">
         <v>301</v>
       </c>
       <c r="E11" s="4" t="s">
@@ -2323,18 +2260,13 @@
       <c r="J11" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="K11" s="23" t="s">
-        <v>349</v>
-      </c>
-      <c r="L11" s="5" t="s">
-        <v>352</v>
-      </c>
+      <c r="K11" s="23"/>
     </row>
     <row r="12" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="56"/>
-      <c r="B12" s="59"/>
-      <c r="C12" s="59"/>
-      <c r="D12" s="59"/>
+      <c r="A12" s="53"/>
+      <c r="B12" s="56"/>
+      <c r="C12" s="56"/>
+      <c r="D12" s="56"/>
       <c r="E12" s="4" t="s">
         <v>119</v>
       </c>
@@ -2353,18 +2285,13 @@
       <c r="J12" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="K12" s="42" t="s">
-        <v>354</v>
-      </c>
-      <c r="L12" s="4" t="s">
-        <v>353</v>
-      </c>
+      <c r="K12" s="39"/>
     </row>
     <row r="13" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="57"/>
-      <c r="B13" s="60"/>
-      <c r="C13" s="60"/>
-      <c r="D13" s="60"/>
+      <c r="A13" s="54"/>
+      <c r="B13" s="57"/>
+      <c r="C13" s="57"/>
+      <c r="D13" s="57"/>
       <c r="E13" s="4" t="s">
         <v>120</v>
       </c>
@@ -2383,12 +2310,7 @@
       <c r="J13" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="K13" s="22" t="s">
-        <v>349</v>
-      </c>
-      <c r="L13" s="38" t="s">
-        <v>352</v>
-      </c>
+      <c r="L13" s="38"/>
     </row>
     <row r="14" spans="1:12" s="5" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A14" s="16">
@@ -2421,12 +2343,7 @@
       <c r="J14" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="K14" s="23" t="s">
-        <v>349</v>
-      </c>
-      <c r="L14" s="5" t="s">
-        <v>355</v>
-      </c>
+      <c r="K14" s="23"/>
     </row>
     <row r="15" spans="1:12" s="5" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A15" s="16">
@@ -2459,12 +2376,7 @@
       <c r="J15" s="18">
         <v>22898</v>
       </c>
-      <c r="K15" s="23" t="s">
-        <v>349</v>
-      </c>
-      <c r="L15" s="5" t="s">
-        <v>356</v>
-      </c>
+      <c r="K15" s="23"/>
     </row>
     <row r="16" spans="1:12" s="5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="16">
@@ -2497,24 +2409,19 @@
       <c r="J16" s="18">
         <v>22459</v>
       </c>
-      <c r="K16" s="23" t="s">
-        <v>349</v>
-      </c>
-      <c r="L16" s="5" t="s">
-        <v>357</v>
-      </c>
+      <c r="K16" s="23"/>
     </row>
-    <row r="17" spans="1:12" s="5" customFormat="1" ht="135" x14ac:dyDescent="0.25">
-      <c r="A17" s="55" t="s">
+    <row r="17" spans="1:11" s="5" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+      <c r="A17" s="52" t="s">
         <v>78</v>
       </c>
-      <c r="B17" s="58" t="s">
+      <c r="B17" s="55" t="s">
         <v>62</v>
       </c>
-      <c r="C17" s="58" t="s">
+      <c r="C17" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="58" t="s">
+      <c r="D17" s="55" t="s">
         <v>305</v>
       </c>
       <c r="E17" s="4" t="s">
@@ -2535,18 +2442,13 @@
       <c r="J17" s="18">
         <v>27778</v>
       </c>
-      <c r="K17" s="23" t="s">
-        <v>349</v>
-      </c>
-      <c r="L17" s="5" t="s">
-        <v>358</v>
-      </c>
+      <c r="K17" s="23"/>
     </row>
-    <row r="18" spans="1:12" ht="135" x14ac:dyDescent="0.25">
-      <c r="A18" s="57"/>
-      <c r="B18" s="60"/>
-      <c r="C18" s="60"/>
-      <c r="D18" s="60"/>
+    <row r="18" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+      <c r="A18" s="54"/>
+      <c r="B18" s="57"/>
+      <c r="C18" s="57"/>
+      <c r="D18" s="57"/>
       <c r="E18" s="4" t="s">
         <v>304</v>
       </c>
@@ -2565,24 +2467,18 @@
       <c r="J18" s="18">
         <v>10132</v>
       </c>
-      <c r="K18" s="22" t="s">
-        <v>349</v>
-      </c>
-      <c r="L18" s="4" t="s">
-        <v>359</v>
-      </c>
     </row>
-    <row r="19" spans="1:12" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="55" t="s">
+    <row r="19" spans="1:11" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" s="52" t="s">
         <v>80</v>
       </c>
-      <c r="B19" s="58" t="s">
+      <c r="B19" s="55" t="s">
         <v>81</v>
       </c>
-      <c r="C19" s="58" t="s">
+      <c r="C19" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="58" t="s">
+      <c r="D19" s="55" t="s">
         <v>4</v>
       </c>
       <c r="E19" s="4" t="s">
@@ -2603,15 +2499,13 @@
       <c r="J19" s="18">
         <v>19136</v>
       </c>
-      <c r="K19" s="23" t="s">
-        <v>349</v>
-      </c>
+      <c r="K19" s="23"/>
     </row>
-    <row r="20" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A20" s="57"/>
-      <c r="B20" s="60"/>
-      <c r="C20" s="60"/>
-      <c r="D20" s="60"/>
+    <row r="20" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="54"/>
+      <c r="B20" s="57"/>
+      <c r="C20" s="57"/>
+      <c r="D20" s="57"/>
       <c r="E20" s="4" t="s">
         <v>122</v>
       </c>
@@ -2630,11 +2524,8 @@
       <c r="J20" s="18">
         <v>10610</v>
       </c>
-      <c r="K20" s="22" t="s">
-        <v>349</v>
-      </c>
     </row>
-    <row r="21" spans="1:12" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
         <v>82</v>
       </c>
@@ -2665,14 +2556,9 @@
       <c r="J21" s="18">
         <v>26580</v>
       </c>
-      <c r="K21" s="23" t="s">
-        <v>349</v>
-      </c>
-      <c r="L21" s="5" t="s">
-        <v>360</v>
-      </c>
+      <c r="K21" s="23"/>
     </row>
-    <row r="22" spans="1:12" s="5" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" s="5" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A22" s="20" t="s">
         <v>255</v>
       </c>
@@ -2703,11 +2589,9 @@
       <c r="J22" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="K22" s="23" t="s">
-        <v>349</v>
-      </c>
+      <c r="K22" s="23"/>
     </row>
-    <row r="23" spans="1:12" s="5" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" s="5" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
         <v>261</v>
       </c>
@@ -2738,11 +2622,9 @@
       <c r="J23" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="K23" s="23" t="s">
-        <v>349</v>
-      </c>
+      <c r="K23" s="23"/>
     </row>
-    <row r="24" spans="1:12" s="29" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" s="29" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="27" t="s">
         <v>308</v>
       </c>
@@ -2773,11 +2655,8 @@
       <c r="J24" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="K24" s="29" t="s">
-        <v>349</v>
-      </c>
     </row>
-    <row r="25" spans="1:12" s="29" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" s="29" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A25" s="27" t="s">
         <v>311</v>
       </c>
@@ -2808,11 +2687,8 @@
       <c r="J25" s="3" t="s">
         <v>325</v>
       </c>
-      <c r="K25" s="29" t="s">
-        <v>349</v>
-      </c>
     </row>
-    <row r="26" spans="1:12" s="29" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" s="29" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A26" s="27" t="s">
         <v>314</v>
       </c>
@@ -2843,16 +2719,13 @@
       <c r="J26" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="K26" s="29" t="s">
-        <v>349</v>
-      </c>
     </row>
-    <row r="27" spans="1:12" s="29" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" s="29" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A27" s="27" t="s">
         <v>318</v>
       </c>
       <c r="B27" s="29" t="s">
-        <v>361</v>
+        <v>350</v>
       </c>
       <c r="C27" s="29" t="s">
         <v>6</v>
@@ -2878,41 +2751,40 @@
       <c r="J27" s="3" t="s">
         <v>331</v>
       </c>
-      <c r="K27" s="29" t="s">
-        <v>349</v>
-      </c>
     </row>
-    <row r="28" spans="1:12" s="40" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="39" t="s">
-        <v>366</v>
-      </c>
-      <c r="B28" s="40" t="s">
-        <v>367</v>
-      </c>
-      <c r="C28" s="40" t="s">
+    <row r="28" spans="1:11" s="47" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="A28" s="46" t="s">
+        <v>353</v>
+      </c>
+      <c r="B28" s="47" t="s">
+        <v>354</v>
+      </c>
+      <c r="C28" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="D28" s="40" t="s">
-        <v>368</v>
-      </c>
-      <c r="E28" s="41"/>
-      <c r="F28">
+      <c r="D28" s="47" t="s">
+        <v>355</v>
+      </c>
+      <c r="E28" s="45" t="s">
+        <v>359</v>
+      </c>
+      <c r="F28" s="17">
         <v>1007953</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G28" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="H28" t="s">
-        <v>369</v>
-      </c>
-      <c r="I28" t="s">
-        <v>370</v>
-      </c>
-      <c r="J28" t="s">
-        <v>371</v>
+      <c r="H28" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>358</v>
       </c>
     </row>
-    <row r="29" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="12">
         <v>2</v>
       </c>
@@ -2923,17 +2795,17 @@
       <c r="D29" s="14"/>
       <c r="E29" s="14"/>
     </row>
-    <row r="30" spans="1:12" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A30" s="55">
+    <row r="30" spans="1:11" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A30" s="52">
         <v>2.1</v>
       </c>
-      <c r="B30" s="58" t="s">
+      <c r="B30" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="C30" s="58" t="s">
+      <c r="C30" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="D30" s="58" t="s">
+      <c r="D30" s="55" t="s">
         <v>46</v>
       </c>
       <c r="E30" s="4" t="s">
@@ -2954,15 +2826,13 @@
       <c r="J30" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="K30" s="23" t="s">
-        <v>349</v>
-      </c>
+      <c r="K30" s="23"/>
     </row>
-    <row r="31" spans="1:12" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A31" s="56"/>
-      <c r="B31" s="59"/>
-      <c r="C31" s="59"/>
-      <c r="D31" s="59"/>
+    <row r="31" spans="1:11" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A31" s="53"/>
+      <c r="B31" s="56"/>
+      <c r="C31" s="56"/>
+      <c r="D31" s="56"/>
       <c r="E31" s="4" t="s">
         <v>123</v>
       </c>
@@ -2981,15 +2851,13 @@
       <c r="J31" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="K31" s="24" t="s">
-        <v>349</v>
-      </c>
+      <c r="K31" s="24"/>
     </row>
-    <row r="32" spans="1:12" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A32" s="57"/>
-      <c r="B32" s="60"/>
-      <c r="C32" s="60"/>
-      <c r="D32" s="60"/>
+    <row r="32" spans="1:11" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A32" s="54"/>
+      <c r="B32" s="57"/>
+      <c r="C32" s="57"/>
+      <c r="D32" s="57"/>
       <c r="E32" s="4" t="s">
         <v>125</v>
       </c>
@@ -3008,21 +2876,19 @@
       <c r="J32" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="K32" s="24" t="s">
-        <v>349</v>
-      </c>
+      <c r="K32" s="24"/>
     </row>
     <row r="33" spans="1:16380" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A33" s="55">
+      <c r="A33" s="52">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B33" s="58" t="s">
+      <c r="B33" s="55" t="s">
         <v>25</v>
       </c>
-      <c r="C33" s="58" t="s">
+      <c r="C33" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="D33" s="58" t="s">
+      <c r="D33" s="55" t="s">
         <v>47</v>
       </c>
       <c r="E33" s="4" t="s">
@@ -3043,15 +2909,13 @@
       <c r="J33" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="K33" s="23" t="s">
-        <v>349</v>
-      </c>
+      <c r="K33" s="23"/>
     </row>
     <row r="34" spans="1:16380" ht="60" x14ac:dyDescent="0.25">
-      <c r="A34" s="57"/>
-      <c r="B34" s="60"/>
-      <c r="C34" s="60"/>
-      <c r="D34" s="60"/>
+      <c r="A34" s="54"/>
+      <c r="B34" s="57"/>
+      <c r="C34" s="57"/>
+      <c r="D34" s="57"/>
       <c r="E34" s="4" t="s">
         <v>129</v>
       </c>
@@ -3070,9 +2934,7 @@
       <c r="J34" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="K34" s="23" t="s">
-        <v>349</v>
-      </c>
+      <c r="K34" s="23"/>
       <c r="L34" s="5"/>
     </row>
     <row r="35" spans="1:16380" s="5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -3106,21 +2968,19 @@
       <c r="J35" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="K35" s="23" t="s">
-        <v>349</v>
-      </c>
+      <c r="K35" s="23"/>
     </row>
     <row r="36" spans="1:16380" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A36" s="55">
+      <c r="A36" s="52">
         <v>2.4</v>
       </c>
-      <c r="B36" s="58" t="s">
+      <c r="B36" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="C36" s="58" t="s">
+      <c r="C36" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="D36" s="58" t="s">
+      <c r="D36" s="55" t="s">
         <v>31</v>
       </c>
       <c r="E36" s="4" t="s">
@@ -3141,15 +3001,13 @@
       <c r="J36" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="K36" s="23" t="s">
-        <v>349</v>
-      </c>
+      <c r="K36" s="23"/>
     </row>
     <row r="37" spans="1:16380" ht="60" x14ac:dyDescent="0.25">
-      <c r="A37" s="56"/>
-      <c r="B37" s="59"/>
-      <c r="C37" s="59"/>
-      <c r="D37" s="59"/>
+      <c r="A37" s="53"/>
+      <c r="B37" s="56"/>
+      <c r="C37" s="56"/>
+      <c r="D37" s="56"/>
       <c r="E37" s="4" t="s">
         <v>127</v>
       </c>
@@ -3168,15 +3026,12 @@
       <c r="J37" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="K37" s="22" t="s">
-        <v>349</v>
-      </c>
     </row>
     <row r="38" spans="1:16380" ht="60" x14ac:dyDescent="0.25">
-      <c r="A38" s="56"/>
-      <c r="B38" s="59"/>
-      <c r="C38" s="59"/>
-      <c r="D38" s="59"/>
+      <c r="A38" s="53"/>
+      <c r="B38" s="56"/>
+      <c r="C38" s="56"/>
+      <c r="D38" s="56"/>
       <c r="E38" s="4" t="s">
         <v>126</v>
       </c>
@@ -3195,15 +3050,12 @@
       <c r="J38" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="K38" s="22" t="s">
-        <v>349</v>
-      </c>
     </row>
     <row r="39" spans="1:16380" ht="60" x14ac:dyDescent="0.25">
-      <c r="A39" s="57"/>
-      <c r="B39" s="60"/>
-      <c r="C39" s="60"/>
-      <c r="D39" s="60"/>
+      <c r="A39" s="54"/>
+      <c r="B39" s="57"/>
+      <c r="C39" s="57"/>
+      <c r="D39" s="57"/>
       <c r="E39" s="4" t="s">
         <v>122</v>
       </c>
@@ -3222,21 +3074,18 @@
       <c r="J39" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="K39" s="22" t="s">
-        <v>349</v>
-      </c>
     </row>
     <row r="40" spans="1:16380" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A40" s="55">
+      <c r="A40" s="52">
         <v>2.5</v>
       </c>
-      <c r="B40" s="58" t="s">
+      <c r="B40" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="C40" s="58" t="s">
+      <c r="C40" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="D40" s="58" t="s">
+      <c r="D40" s="55" t="s">
         <v>49</v>
       </c>
       <c r="E40" s="4" t="s">
@@ -3257,16 +3106,14 @@
       <c r="J40" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="K40" s="22" t="s">
-        <v>349</v>
-      </c>
+      <c r="K40" s="22"/>
       <c r="L40" s="4"/>
     </row>
     <row r="41" spans="1:16380" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A41" s="57"/>
-      <c r="B41" s="60"/>
-      <c r="C41" s="60"/>
-      <c r="D41" s="60"/>
+      <c r="A41" s="54"/>
+      <c r="B41" s="57"/>
+      <c r="C41" s="57"/>
+      <c r="D41" s="57"/>
       <c r="E41" s="4" t="s">
         <v>132</v>
       </c>
@@ -3285,12 +3132,10 @@
       <c r="J41" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="K41" s="22" t="s">
-        <v>349</v>
-      </c>
+      <c r="K41" s="22"/>
       <c r="L41" s="4"/>
     </row>
-    <row r="42" spans="1:16380" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16380" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="30" t="s">
         <v>252</v>
       </c>
@@ -19711,9 +19556,7 @@
       <c r="J43" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="K43" s="23" t="s">
-        <v>349</v>
-      </c>
+      <c r="K43" s="23"/>
     </row>
     <row r="44" spans="1:16380" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="12">
@@ -19726,7 +19569,7 @@
       <c r="D44" s="14"/>
       <c r="E44" s="14"/>
     </row>
-    <row r="45" spans="1:16380" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16380" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A45" s="30">
         <v>3.1</v>
       </c>
@@ -36129,16 +35972,16 @@
       <c r="XEZ45" s="29"/>
     </row>
     <row r="46" spans="1:16380" s="33" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A46" s="50">
+      <c r="A46" s="60">
         <v>3.2</v>
       </c>
-      <c r="B46" s="52" t="s">
+      <c r="B46" s="62" t="s">
         <v>107</v>
       </c>
-      <c r="C46" s="54" t="s">
+      <c r="C46" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="D46" s="52" t="s">
+      <c r="D46" s="62" t="s">
         <v>33</v>
       </c>
       <c r="E46" s="32" t="s">
@@ -36161,10 +36004,10 @@
       </c>
     </row>
     <row r="47" spans="1:16380" s="32" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A47" s="51"/>
-      <c r="B47" s="53"/>
-      <c r="C47" s="53"/>
-      <c r="D47" s="53"/>
+      <c r="A47" s="61"/>
+      <c r="B47" s="63"/>
+      <c r="C47" s="63"/>
+      <c r="D47" s="63"/>
       <c r="E47" s="32" t="s">
         <v>134</v>
       </c>
@@ -36184,7 +36027,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="48" spans="1:16380" s="31" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16380" s="31" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A48" s="30">
         <v>3.3</v>
       </c>
@@ -36217,16 +36060,16 @@
       </c>
     </row>
     <row r="49" spans="1:12" s="33" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A49" s="50" t="s">
+      <c r="A49" s="60" t="s">
         <v>96</v>
       </c>
-      <c r="B49" s="52" t="s">
+      <c r="B49" s="62" t="s">
         <v>103</v>
       </c>
-      <c r="C49" s="52" t="s">
+      <c r="C49" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="D49" s="52" t="s">
+      <c r="D49" s="62" t="s">
         <v>136</v>
       </c>
       <c r="E49" s="32" t="s">
@@ -36249,10 +36092,10 @@
       </c>
     </row>
     <row r="50" spans="1:12" s="32" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A50" s="51"/>
-      <c r="B50" s="53"/>
-      <c r="C50" s="53"/>
-      <c r="D50" s="53"/>
+      <c r="A50" s="61"/>
+      <c r="B50" s="63"/>
+      <c r="C50" s="63"/>
+      <c r="D50" s="63"/>
       <c r="E50" s="32" t="s">
         <v>125</v>
       </c>
@@ -36272,7 +36115,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="51" spans="1:12" s="35" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" s="35" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A51" s="34" t="s">
         <v>97</v>
       </c>
@@ -36304,7 +36147,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="52" spans="1:12" s="35" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" s="35" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A52" s="34" t="s">
         <v>98</v>
       </c>
@@ -36367,9 +36210,7 @@
       <c r="J53" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="K53" s="23" t="s">
-        <v>349</v>
-      </c>
+      <c r="K53" s="23"/>
     </row>
     <row r="54" spans="1:12" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A54" s="16" t="s">
@@ -36402,12 +36243,7 @@
       <c r="J54" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="K54" s="23" t="s">
-        <v>349</v>
-      </c>
-      <c r="L54" s="5" t="s">
-        <v>362</v>
-      </c>
+      <c r="K54" s="23"/>
     </row>
     <row r="55" spans="1:12" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A55" s="19" t="s">
@@ -36440,66 +36276,60 @@
       <c r="J55" t="s">
         <v>271</v>
       </c>
-      <c r="K55" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="L55" s="1" t="s">
-        <v>362</v>
-      </c>
     </row>
-    <row r="56" spans="1:12" s="46" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A56" s="49" t="s">
+    <row r="56" spans="1:12" s="43" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A56" s="59" t="s">
         <v>91</v>
       </c>
-      <c r="B56" s="48" t="s">
+      <c r="B56" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="C56" s="48" t="s">
+      <c r="C56" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="D56" s="48" t="s">
+      <c r="D56" s="58" t="s">
         <v>73</v>
       </c>
-      <c r="E56" s="43" t="s">
+      <c r="E56" s="40" t="s">
         <v>135</v>
       </c>
-      <c r="F56" s="44">
+      <c r="F56" s="41">
         <v>1007922</v>
       </c>
-      <c r="G56" s="45" t="s">
+      <c r="G56" s="42" t="s">
         <v>153</v>
       </c>
-      <c r="H56" s="45" t="s">
+      <c r="H56" s="42" t="s">
         <v>169</v>
       </c>
-      <c r="I56" s="45" t="s">
+      <c r="I56" s="42" t="s">
         <v>170</v>
       </c>
-      <c r="J56" s="45" t="s">
+      <c r="J56" s="42" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="57" spans="1:12" s="46" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A57" s="49"/>
-      <c r="B57" s="48"/>
-      <c r="C57" s="48"/>
-      <c r="D57" s="48"/>
-      <c r="E57" s="45" t="s">
+    <row r="57" spans="1:12" s="43" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A57" s="59"/>
+      <c r="B57" s="58"/>
+      <c r="C57" s="58"/>
+      <c r="D57" s="58"/>
+      <c r="E57" s="42" t="s">
         <v>134</v>
       </c>
-      <c r="F57" s="44">
+      <c r="F57" s="41">
         <v>1007913</v>
       </c>
-      <c r="G57" s="45" t="s">
+      <c r="G57" s="42" t="s">
         <v>142</v>
       </c>
-      <c r="H57" s="45" t="s">
+      <c r="H57" s="42" t="s">
         <v>145</v>
       </c>
-      <c r="I57" s="45" t="s">
+      <c r="I57" s="42" t="s">
         <v>146</v>
       </c>
-      <c r="J57" s="45" t="s">
+      <c r="J57" s="42" t="s">
         <v>147</v>
       </c>
     </row>
@@ -36531,12 +36361,8 @@
       <c r="J58" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="K58" s="42" t="s">
-        <v>354</v>
-      </c>
-      <c r="L58" s="37" t="s">
-        <v>353</v>
-      </c>
+      <c r="K58" s="39"/>
+      <c r="L58" s="37"/>
     </row>
     <row r="59" spans="1:12" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A59" s="16" t="s">
@@ -36566,12 +36392,7 @@
       <c r="J59" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="K59" s="23" t="s">
-        <v>349</v>
-      </c>
-      <c r="L59" s="5" t="s">
-        <v>363</v>
-      </c>
+      <c r="K59" s="23"/>
     </row>
     <row r="60" spans="1:12" s="5" customFormat="1" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="16" t="s">
@@ -36601,14 +36422,10 @@
       <c r="J60" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="K60" s="23" t="s">
-        <v>349</v>
-      </c>
-      <c r="L60" s="1" t="s">
-        <v>362</v>
-      </c>
+      <c r="K60" s="23"/>
+      <c r="L60" s="1"/>
     </row>
-    <row r="61" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="12">
         <v>4</v>
       </c>
@@ -36650,21 +36467,18 @@
       <c r="J62" t="s">
         <v>268</v>
       </c>
-      <c r="K62" s="22" t="s">
-        <v>349</v>
-      </c>
     </row>
-    <row r="63" spans="1:12" s="45" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="47">
+    <row r="63" spans="1:12" s="42" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A63" s="44">
         <v>4.2</v>
       </c>
-      <c r="B63" s="45" t="s">
+      <c r="B63" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="C63" s="45" t="s">
+      <c r="C63" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="D63" s="45" t="s">
+      <c r="D63" s="42" t="s">
         <v>56</v>
       </c>
     </row>
@@ -36699,11 +36513,8 @@
       <c r="J64" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="K64" s="22" t="s">
-        <v>349</v>
-      </c>
     </row>
-    <row r="65" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A65" s="8">
         <v>4.4000000000000004</v>
       </c>
@@ -36734,11 +36545,8 @@
       <c r="J65" t="s">
         <v>274</v>
       </c>
-      <c r="K65" s="22" t="s">
-        <v>349</v>
-      </c>
     </row>
-    <row r="66" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A66" s="8">
         <v>4.5</v>
       </c>
@@ -36769,11 +36577,8 @@
       <c r="J66" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="K66" s="22" t="s">
-        <v>349</v>
-      </c>
     </row>
-    <row r="67" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A67" s="8">
         <v>4.5999999999999996</v>
       </c>
@@ -36804,16 +36609,13 @@
       <c r="J67" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="K67" s="22" t="s">
-        <v>349</v>
-      </c>
     </row>
-    <row r="68" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A68" s="8">
         <v>4.7</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>364</v>
+        <v>351</v>
       </c>
       <c r="C68" s="4" t="s">
         <v>6</v>
@@ -36839,16 +36641,13 @@
       <c r="J68" t="s">
         <v>277</v>
       </c>
-      <c r="K68" s="22" t="s">
-        <v>349</v>
-      </c>
     </row>
-    <row r="69" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A69" s="8">
         <v>4.8</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>365</v>
+        <v>352</v>
       </c>
       <c r="C69" s="4" t="s">
         <v>6</v>
@@ -36874,11 +36673,8 @@
       <c r="J69" t="s">
         <v>274</v>
       </c>
-      <c r="K69" s="22" t="s">
-        <v>349</v>
-      </c>
     </row>
-    <row r="70" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="12">
         <v>5</v>
       </c>
@@ -36889,7 +36685,7 @@
       <c r="D70" s="14"/>
       <c r="E70" s="14"/>
     </row>
-    <row r="71" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A71" s="8">
         <v>5.0999999999999996</v>
       </c>
@@ -36920,11 +36716,8 @@
       <c r="J71" t="s">
         <v>280</v>
       </c>
-      <c r="K71" s="22" t="s">
-        <v>349</v>
-      </c>
     </row>
-    <row r="72" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A72" s="8">
         <v>5.2</v>
       </c>
@@ -36955,11 +36748,8 @@
       <c r="J72" t="s">
         <v>283</v>
       </c>
-      <c r="K72" s="22" t="s">
-        <v>349</v>
-      </c>
     </row>
-    <row r="73" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A73" s="8">
         <v>5.3</v>
       </c>
@@ -36990,11 +36780,8 @@
       <c r="J73" t="s">
         <v>285</v>
       </c>
-      <c r="K73" s="22" t="s">
-        <v>349</v>
-      </c>
     </row>
-    <row r="74" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" s="12">
         <v>6</v>
       </c>
@@ -37005,7 +36792,7 @@
       <c r="D74" s="14"/>
       <c r="E74" s="14"/>
     </row>
-    <row r="75" spans="1:11" s="32" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" s="32" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A75" s="36">
         <v>6.1</v>
       </c>
@@ -37026,7 +36813,7 @@
       <c r="I75" s="4"/>
       <c r="J75" s="4"/>
     </row>
-    <row r="76" spans="1:11" s="32" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" s="32" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A76" s="36">
         <v>6.2</v>
       </c>
@@ -37047,7 +36834,7 @@
       <c r="I76" s="4"/>
       <c r="J76" s="4"/>
     </row>
-    <row r="77" spans="1:11" s="32" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" s="32" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A77" s="36">
         <v>6.3</v>
       </c>
@@ -37068,7 +36855,7 @@
       <c r="I77" s="4"/>
       <c r="J77" s="4"/>
     </row>
-    <row r="78" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="12">
         <v>7</v>
       </c>
@@ -37079,7 +36866,7 @@
       <c r="D78" s="14"/>
       <c r="E78" s="14"/>
     </row>
-    <row r="79" spans="1:11" s="32" customFormat="1" ht="240" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" s="32" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A79" s="36">
         <v>7.1</v>
       </c>
@@ -37094,7 +36881,7 @@
       <c r="I79" s="4"/>
       <c r="J79" s="4"/>
     </row>
-    <row r="80" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="12" t="s">
         <v>332</v>
       </c>
@@ -37125,7 +36912,7 @@
         <v>1008005</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A82" s="8" t="s">
         <v>337</v>
       </c>
@@ -37142,7 +36929,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" ht="180" x14ac:dyDescent="0.25">
       <c r="A83" s="26" t="s">
         <v>340</v>
       </c>
@@ -37159,7 +36946,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="84" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A84" s="8" t="s">
         <v>343</v>
       </c>
@@ -37176,7 +36963,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="85" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A85" s="26" t="s">
         <v>346</v>
       </c>
@@ -37196,38 +36983,6 @@
   </sheetData>
   <autoFilter ref="A3:J85"/>
   <mergeCells count="44">
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="D11:D13"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="B30:B32"/>
-    <mergeCell ref="C30:C32"/>
-    <mergeCell ref="D30:D32"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="B36:B39"/>
-    <mergeCell ref="C36:C39"/>
-    <mergeCell ref="D36:D39"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="D40:D41"/>
     <mergeCell ref="D56:D57"/>
     <mergeCell ref="C56:C57"/>
     <mergeCell ref="B56:B57"/>
@@ -37240,6 +36995,38 @@
     <mergeCell ref="B49:B50"/>
     <mergeCell ref="C49:C50"/>
     <mergeCell ref="D49:D50"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="B36:B39"/>
+    <mergeCell ref="C36:C39"/>
+    <mergeCell ref="D36:D39"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="C30:C32"/>
+    <mergeCell ref="D30:D32"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="D11:D13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="14" orientation="landscape" r:id="rId1"/>

</xml_diff>